<commit_message>
update import export excel
</commit_message>
<xml_diff>
--- a/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/EmployeeTemplate.xlsx
+++ b/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/EmployeeTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git-Responsitory\DotNet\ASP.NET CORE\HRMNS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\Source\NET CORE\ASP.NET CORE\HRMNS\HRMS\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>STT</t>
   </si>
@@ -130,13 +130,76 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>H2205001</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>Lê Văn Đặng</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Thôn Phúc Long, xã Tăng Tiến, huyện Việt Yên, Tỉnh Bắc Giang</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>Kinh</t>
+  </si>
+  <si>
+    <t>Số 23, ngõ 394, đường Mỹ Đình, Nam Từ Liêm, Hà Nội</t>
+  </si>
+  <si>
+    <t>danglevan.9919@gmail.com</t>
+  </si>
+  <si>
+    <t>0974628108</t>
+  </si>
+  <si>
+    <t>09123123123</t>
+  </si>
+  <si>
+    <t>Em Trai</t>
+  </si>
+  <si>
+    <t>Công An Tỉnh Băc Giang</t>
+  </si>
+  <si>
+    <t>SHIN HAN BANK</t>
+  </si>
+  <si>
+    <t>123214123123123</t>
+  </si>
+  <si>
+    <t>Học viện kỹ thuật quân sự</t>
+  </si>
+  <si>
+    <t>Không</t>
+  </si>
+  <si>
+    <t>123123123123</t>
+  </si>
+  <si>
+    <t>98123123123</t>
+  </si>
+  <si>
+    <t>Tôn giáo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +217,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -259,36 +330,49 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
@@ -568,175 +652,252 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AD3" sqref="AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="2" t="s">
+      <c r="O1" s="13"/>
+      <c r="P1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="AD1" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="2" spans="1:29" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="5" t="s">
+    <row r="2" spans="1:30" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
+    <row r="3" spans="1:30" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="3">
+        <v>44586</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="2">
+        <v>122029039</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>44586</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V3" s="3">
+        <v>44586</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="AA1:AC2" name="Range1_3" securityDescriptor="O:WDG:WDD:(A;;CC;;;BU)"/>
+    <protectedRange sqref="AA1:AD2" name="Range1_3" securityDescriptor="O:WDG:WDD:(A;;CC;;;BU)"/>
   </protectedRanges>
-  <mergeCells count="28">
+  <mergeCells count="29">
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
     <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="AC1:AC2"/>
     <mergeCell ref="S1:S2"/>
@@ -753,19 +914,11 @@
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="U1:U2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="L3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update nhan vien: upload file and review
</commit_message>
<xml_diff>
--- a/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/EmployeeTemplate.xlsx
+++ b/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/EmployeeTemplate.xlsx
@@ -13,6 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="2" r:id="rId1"/>
+    <sheet name="BoPhans" sheetId="3" r:id="rId2"/>
+    <sheet name="Chuc Danh" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
   <si>
     <t>STT</t>
   </si>
@@ -111,12 +113,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>số sổ BH</t>
-  </si>
-  <si>
-    <t>mã số thuế</t>
-  </si>
-  <si>
     <t>Số người giảm trừ</t>
   </si>
   <si>
@@ -138,9 +134,6 @@
     <t>Staff</t>
   </si>
   <si>
-    <t>PI</t>
-  </si>
-  <si>
     <t>Lê Văn Đặng</t>
   </si>
   <si>
@@ -174,9 +167,6 @@
     <t>Công An Tỉnh Băc Giang</t>
   </si>
   <si>
-    <t>SHIN HAN BANK</t>
-  </si>
-  <si>
     <t>123214123123123</t>
   </si>
   <si>
@@ -193,6 +183,181 @@
   </si>
   <si>
     <t>Tôn giáo</t>
+  </si>
+  <si>
+    <t>CSP</t>
+  </si>
+  <si>
+    <t>KHO</t>
+  </si>
+  <si>
+    <t>KOREA</t>
+  </si>
+  <si>
+    <t>LFEM</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t>SMT</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>UTILITY</t>
+  </si>
+  <si>
+    <t>WLP1</t>
+  </si>
+  <si>
+    <t>WLP2</t>
+  </si>
+  <si>
+    <t>Assistant leader</t>
+  </si>
+  <si>
+    <t>Assistant leader/ Phó nhóm</t>
+  </si>
+  <si>
+    <t>Assistant Manager</t>
+  </si>
+  <si>
+    <t>Engineer Assistant leader</t>
+  </si>
+  <si>
+    <t>Engineer Assistant leader/ Phó nhóm kỹ thuật</t>
+  </si>
+  <si>
+    <t>Engineer shift leader</t>
+  </si>
+  <si>
+    <t>Engineer shift leader/ Tổ trưởng kỹ thuật</t>
+  </si>
+  <si>
+    <t>Engineer supervisor</t>
+  </si>
+  <si>
+    <t>Engineer supervisor/ Giám sát kỹ thuật</t>
+  </si>
+  <si>
+    <t>General Director</t>
+  </si>
+  <si>
+    <t>General Manager</t>
+  </si>
+  <si>
+    <t>Group Leader</t>
+  </si>
+  <si>
+    <t>Group Leader/ Trưởng bộ phận</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Operator</t>
+  </si>
+  <si>
+    <t>Operator/ Công nhân</t>
+  </si>
+  <si>
+    <t>Operator Radiation safety</t>
+  </si>
+  <si>
+    <t>Operator/ Công nhân - An toàn bức xạ</t>
+  </si>
+  <si>
+    <t>Operator TOXIC</t>
+  </si>
+  <si>
+    <t>Operator/ Công nhân tiếp xúc hóa chất độc hại</t>
+  </si>
+  <si>
+    <t>Operator XRF</t>
+  </si>
+  <si>
+    <t>Operator/ Công nhân (bức xạ XRF)</t>
+  </si>
+  <si>
+    <t>Part Leader</t>
+  </si>
+  <si>
+    <t>Part Leader/ Trưởng nhóm</t>
+  </si>
+  <si>
+    <t>Senior Manager</t>
+  </si>
+  <si>
+    <t>Shift leader</t>
+  </si>
+  <si>
+    <t>Shift leader/ Tổ trưởng sản xuất</t>
+  </si>
+  <si>
+    <t>Staff Ma</t>
+  </si>
+  <si>
+    <t>Staff/ Nhân viên - Mạ</t>
+  </si>
+  <si>
+    <t>Staff Reveal</t>
+  </si>
+  <si>
+    <t>Staff/ Nhân viên - Lộ quang</t>
+  </si>
+  <si>
+    <t>Staff Xray</t>
+  </si>
+  <si>
+    <t>Staff/ Nhân viên - Bức xạ máy Xray</t>
+  </si>
+  <si>
+    <t>Staff XRF</t>
+  </si>
+  <si>
+    <t>Staff/ Nhân viên (bức xạ XRF)</t>
+  </si>
+  <si>
+    <t>Supervisor</t>
+  </si>
+  <si>
+    <t>Supervisor/ Giám sát line</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Tinh Trang Hon Nhan</t>
+  </si>
+  <si>
+    <t>SHINHAN BANK</t>
+  </si>
+  <si>
+    <t>Ngày Tham Gia BH</t>
+  </si>
+  <si>
+    <t>Ngày Hết Hạn BH</t>
+  </si>
+  <si>
+    <t>Số sổ BH</t>
+  </si>
+  <si>
+    <t>Mã số thuế</t>
+  </si>
+  <si>
+    <t>Tổng phép năm
+(hiện tại)</t>
+  </si>
+  <si>
+    <t>Còn lại  phép năm(hiện tại)</t>
   </si>
 </sst>
 </file>
@@ -227,7 +392,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,6 +402,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,7 +506,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -358,7 +529,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -367,9 +546,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -652,189 +832,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
     <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="34" max="34" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="11" t="s">
+      <c r="L1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="13"/>
-      <c r="P1" s="11" t="s">
+      <c r="O1" s="14"/>
+      <c r="P1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="T1" s="11" t="s">
+      <c r="S1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="V1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AA1" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AF1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="O2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-    </row>
-    <row r="3" spans="1:30" ht="75" x14ac:dyDescent="0.25">
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="13"/>
+    </row>
+    <row r="3" spans="1:34" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="G3" s="3">
         <v>44586</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="L3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="M3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="N3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="O3" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="P3" s="2">
         <v>122029039</v>
@@ -843,49 +1040,63 @@
         <v>44586</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="V3" s="3">
         <v>44586</v>
       </c>
       <c r="W3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="X3" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="Y3" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="Z3" s="2"/>
       <c r="AA3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC3" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB3" s="18">
+        <v>44216</v>
+      </c>
+      <c r="AC3" s="18">
+        <v>44217</v>
+      </c>
+      <c r="AD3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE3" s="11">
         <v>0</v>
       </c>
-      <c r="AD3" s="2" t="s">
-        <v>47</v>
+      <c r="AF3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>12</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="AA1:AD2" name="Range1_3" securityDescriptor="O:WDG:WDD:(A;;CC;;;BU)"/>
+    <protectedRange sqref="AA1:AH2" name="Range1_3" securityDescriptor="O:WDG:WDD:(A;;CC;;;BU)"/>
   </protectedRanges>
-  <mergeCells count="29">
-    <mergeCell ref="AD1:AD2"/>
+  <mergeCells count="31">
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -898,8 +1109,8 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="AD1:AD2"/>
+    <mergeCell ref="AE1:AE2"/>
     <mergeCell ref="S1:S2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="V1:V2"/>
@@ -920,5 +1131,341 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>BoPhans!$A$1:$A$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Chuc Danh'!$A$2:$A$23</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Chuc Danh'!$E$2:$E$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>I3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update import bo phan chi tiet
</commit_message>
<xml_diff>
--- a/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/EmployeeTemplate.xlsx
+++ b/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/EmployeeTemplate.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="133">
   <si>
     <t>STT</t>
   </si>
@@ -358,6 +358,90 @@
   </si>
   <si>
     <t>Còn lại  phép năm(hiện tại)</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Quality Control/ QL Chất lượng (PQC)</t>
+  </si>
+  <si>
+    <t>Quality Control/ QL Chất lượng (QQC)</t>
+  </si>
+  <si>
+    <t>Quality Control/ QL Chất lượng (Reability)</t>
+  </si>
+  <si>
+    <t>SMT Manufacturing/ Sản xuất SMT</t>
+  </si>
+  <si>
+    <t>SMT Innovation Group</t>
+  </si>
+  <si>
+    <t>WLP2 Manufacturing/ Sản xuất WLP2</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
+  </si>
+  <si>
+    <t>WLP1 Manufacturing/ Sản xuất WLP1</t>
+  </si>
+  <si>
+    <t>WLP1 Technology/ Kỹ thuật WLP1</t>
+  </si>
+  <si>
+    <t>WLP2 Technology/ Kỹ thuật WLP2</t>
+  </si>
+  <si>
+    <t>Quality Control/ QL Chất lượng (OQC)</t>
+  </si>
+  <si>
+    <t>SMT Technology/ Kỹ thuật SMT</t>
+  </si>
+  <si>
+    <t>Quality Control/ QL Chất lượng (CS)</t>
+  </si>
+  <si>
+    <t>Quality Control/ QL Chất lượng (IQC)</t>
+  </si>
+  <si>
+    <t>Purchasing/ Mua hàng</t>
+  </si>
+  <si>
+    <t>Quality Control/ QL Chất lượng</t>
+  </si>
+  <si>
+    <t>Accounting/ Kế toán</t>
+  </si>
+  <si>
+    <t>CSP Technology/ Kỹ thuật CSP</t>
+  </si>
+  <si>
+    <t>GOC</t>
+  </si>
+  <si>
+    <t>Human Resource/ HCNS</t>
+  </si>
+  <si>
+    <t>Human Resource/ HCNS (EHS)</t>
+  </si>
+  <si>
+    <t>CSP Manufacturing/ Sản xuất CSP</t>
+  </si>
+  <si>
+    <t>LFEM  Manufacturing/ Sản xuất LFEM</t>
+  </si>
+  <si>
+    <t>LFEM Technology/ Kỹ thuật LFEM</t>
+  </si>
+  <si>
+    <t>Logistic/ XNK</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>Human Resource/ HCNS (Utility)</t>
   </si>
 </sst>
 </file>
@@ -392,7 +476,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,6 +492,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -506,7 +596,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -531,13 +621,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -549,7 +637,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -832,10 +941,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH3"/>
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:AI3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,17 +957,17 @@
     <col min="34" max="34" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="15" t="s">
@@ -870,7 +982,7 @@
       <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="23" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="15" t="s">
@@ -879,16 +991,16 @@
       <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="13" t="s">
         <v>27</v>
       </c>
       <c r="M1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="14"/>
+      <c r="O1" s="18"/>
       <c r="P1" s="15" t="s">
         <v>13</v>
       </c>
@@ -898,7 +1010,7 @@
       <c r="R1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="13" t="s">
         <v>26</v>
       </c>
       <c r="T1" s="15" t="s">
@@ -910,49 +1022,52 @@
       <c r="V1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="W1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="X1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Y1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="Z1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="12" t="s">
+      <c r="AA1" s="13" t="s">
         <v>101</v>
       </c>
       <c r="AB1" s="8"/>
       <c r="AC1" s="8"/>
-      <c r="AD1" s="12" t="s">
+      <c r="AD1" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AE1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AF1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="AG1" s="12" t="s">
+      <c r="AG1" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="AH1" s="12" t="s">
+      <c r="AH1" s="13" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI1" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
+      <c r="I2" s="24"/>
       <c r="J2" s="16"/>
       <c r="K2" s="16"/>
       <c r="L2" s="17"/>
@@ -970,24 +1085,25 @@
       <c r="T2" s="16"/>
       <c r="U2" s="16"/>
       <c r="V2" s="16"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
       <c r="AB2" s="9" t="s">
         <v>99</v>
       </c>
       <c r="AC2" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="13"/>
-      <c r="AF2" s="13"/>
-      <c r="AG2" s="13"/>
-      <c r="AH2" s="13"/>
-    </row>
-    <row r="3" spans="1:34" ht="75" x14ac:dyDescent="0.25">
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="22"/>
+    </row>
+    <row r="3" spans="1:35" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1067,10 +1183,10 @@
       <c r="AA3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AB3" s="18">
+      <c r="AB3" s="12">
         <v>44216</v>
       </c>
-      <c r="AC3" s="18">
+      <c r="AC3" s="12">
         <v>44217</v>
       </c>
       <c r="AD3" s="6" t="s">
@@ -1088,12 +1204,31 @@
       <c r="AH3" s="2">
         <v>9</v>
       </c>
+      <c r="AI3" s="2" t="s">
+        <v>131</v>
+      </c>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="AA1:AH2" name="Range1_3" securityDescriptor="O:WDG:WDD:(A;;CC;;;BU)"/>
+    <protectedRange sqref="AA1:AI2" name="Range1_3" securityDescriptor="O:WDG:WDD:(A;;CC;;;BU)"/>
   </protectedRanges>
-  <mergeCells count="31">
+  <mergeCells count="32">
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Z1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
     <mergeCell ref="AG1:AG2"/>
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AF1:AF2"/>
@@ -1110,21 +1245,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="AD1:AD2"/>
-    <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="Z1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L3" r:id="rId1"/>
@@ -1133,7 +1253,7 @@
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>BoPhans!$A$1:$A$10</xm:f>
@@ -1152,6 +1272,12 @@
           </x14:formula1>
           <xm:sqref>I3</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Chuc Danh'!$I$2:$I$29</xm:f>
+          </x14:formula1>
+          <xm:sqref>AI3</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1160,6 +1286,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="6" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1259,20 +1388,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <sheetPr>
+    <tabColor theme="2" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="2" width="44.85546875" customWidth="1"/>
     <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="8" max="9" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>94</v>
       </c>
@@ -1282,8 +1415,14 @@
       <c r="E1" s="10" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -1293,8 +1432,14 @@
       <c r="E2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" s="19">
+        <v>85</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1304,165 +1449,339 @@
       <c r="E3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H3" s="19">
+        <v>86</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
       <c r="B4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H4" s="19">
+        <v>87</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>62</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H5" s="19">
+        <v>88</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
       <c r="B6" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H6" s="19">
+        <v>89</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>66</v>
       </c>
       <c r="B7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H7" s="19">
+        <v>90</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
       <c r="B8" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H8" s="19">
+        <v>91</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H9" s="19">
+        <v>92</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H10" s="19">
+        <v>93</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>71</v>
       </c>
       <c r="B11" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H11" s="19">
+        <v>94</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>73</v>
       </c>
       <c r="B12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H12" s="19">
+        <v>95</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>75</v>
       </c>
       <c r="B13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H13" s="19">
+        <v>96</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
       <c r="B14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H14" s="19">
+        <v>97</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>79</v>
       </c>
       <c r="B15" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H15" s="19">
+        <v>98</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
       <c r="B16" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H16" s="19">
+        <v>99</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>82</v>
       </c>
       <c r="B17" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H17" s="19">
+        <v>100</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
       <c r="B18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H18" s="19">
+        <v>101</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>84</v>
       </c>
       <c r="B19" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H19" s="19">
+        <v>102</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>86</v>
       </c>
       <c r="B20" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H20" s="19">
+        <v>103</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>88</v>
       </c>
       <c r="B21" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H21" s="19">
+        <v>104</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>90</v>
       </c>
       <c r="B22" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H22" s="19">
+        <v>105</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>92</v>
       </c>
       <c r="B23" t="s">
         <v>93</v>
+      </c>
+      <c r="H23" s="19">
+        <v>106</v>
+      </c>
+      <c r="I23" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="19">
+        <v>107</v>
+      </c>
+      <c r="I24" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="19">
+        <v>108</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="19">
+        <v>109</v>
+      </c>
+      <c r="I26" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H27" s="19">
+        <v>110</v>
+      </c>
+      <c r="I27" s="19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="19">
+        <v>111</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="19">
+        <v>112</v>
+      </c>
+      <c r="I29" s="19" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update Project operation mns, hrmsn, voc
</commit_message>
<xml_diff>
--- a/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/EmployeeTemplate.xlsx
+++ b/ASP.NET CORE/HRMNS/HRMS/wwwroot/templates/EmployeeTemplate.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="141">
   <si>
     <t>STT</t>
   </si>
@@ -469,6 +469,15 @@
       </rPr>
       <t>(YYYY-MM-DD)</t>
     </r>
+  </si>
+  <si>
+    <t>Nơi Tuyển Dụng</t>
+  </si>
+  <si>
+    <t>VN</t>
+  </si>
+  <si>
+    <t>HQ</t>
   </si>
 </sst>
 </file>
@@ -663,10 +672,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -675,16 +684,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -696,10 +699,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -987,10 +996,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:AJ3"/>
+  <dimension ref="A1:AK3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AJ10" sqref="AJ10"/>
+      <selection activeCell="AJ11" sqref="AJ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,69 +1010,69 @@
     <col min="36" max="36" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="18" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="21"/>
-      <c r="P1" s="19" t="s">
+      <c r="O1" s="26"/>
+      <c r="P1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="R1" s="18" t="s">
         <v>15</v>
       </c>
       <c r="S1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="T1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="U1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="V1" s="18" t="s">
         <v>18</v>
       </c>
       <c r="W1" s="16" t="s">
@@ -1098,40 +1107,43 @@
       <c r="AH1" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="AI1" s="14" t="s">
+      <c r="AI1" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="AJ1" s="25" t="s">
+      <c r="AJ1" s="14" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="2" spans="1:36" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="20"/>
+      <c r="AK1" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="19"/>
       <c r="N2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
       <c r="W2" s="17"/>
       <c r="X2" s="17"/>
       <c r="Y2" s="17"/>
@@ -1148,10 +1160,11 @@
       <c r="AF2" s="17"/>
       <c r="AG2" s="17"/>
       <c r="AH2" s="17"/>
-      <c r="AI2" s="15"/>
-      <c r="AJ2" s="26"/>
-    </row>
-    <row r="3" spans="1:36" ht="75" x14ac:dyDescent="0.25">
+      <c r="AI2" s="24"/>
+      <c r="AJ2" s="15"/>
+      <c r="AK2" s="17"/>
+    </row>
+    <row r="3" spans="1:37" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1257,28 +1270,17 @@
       </c>
       <c r="AJ3" s="3">
         <v>44562</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
   <protectedRanges>
     <protectedRange sqref="AA1:AI2" name="Range1_3" securityDescriptor="O:WDG:WDD:(A;;CC;;;BU)"/>
   </protectedRanges>
-  <mergeCells count="33">
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AF1:AF2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
+  <mergeCells count="34">
+    <mergeCell ref="AK1:AK2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="AD1:AD2"/>
     <mergeCell ref="AI1:AI2"/>
@@ -1295,6 +1297,21 @@
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:R2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="M1:M2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="U1:U2"/>
   </mergeCells>
@@ -1302,10 +1319,10 @@
     <hyperlink ref="L3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>BoPhans!$A$1:$A$10</xm:f>
@@ -1330,6 +1347,12 @@
           </x14:formula1>
           <xm:sqref>AI3</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>BoPhans!$A$14:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>AK3</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1341,10 +1364,10 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,6 +1454,16 @@
       </c>
       <c r="B10" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>